<commit_message>
converted test project to actual unit test
</commit_message>
<xml_diff>
--- a/EPPlus.Html.Test/Resources/Test001.xlsx
+++ b/EPPlus.Html.Test/Resources/Test001.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tw\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adkerti\Source\Repos\EPPlus.Html\EPPlus.Html.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B4646E83-C60B-43C4-821A-EF4D18C36297}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff Report" sheetId="1" r:id="rId1"/>
@@ -183,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -239,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -247,9 +248,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -265,7 +269,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -560,19 +564,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="6" width="12.42578125" customWidth="1"/>
+    <col min="4" max="6" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -605,7 +609,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3"/>
@@ -1966,5 +1970,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>